<commit_message>
update model and simulations
</commit_message>
<xml_diff>
--- a/ReconstructionAndAnalysis/suppdata/s3model.xlsx
+++ b/ReconstructionAndAnalysis/suppdata/s3model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\St. Elmo\Dropbox\Research\Writing\iNlan20\Reconstruction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\St. Elmo\Dropbox\Research\Writing\iNlan20\iNlan20\ReconstructionAndAnalysis\suppdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F39679-DAE7-4D25-9653-C0EC53142540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CC1F87-E71E-4773-853D-B24635748A00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23760" yWindow="2175" windowWidth="17280" windowHeight="8970" firstSheet="9" activeTab="13" xr2:uid="{9E3F4571-95A0-4D9B-935E-6906F522B3C5}"/>
+    <workbookView xWindow="-22215" yWindow="1530" windowWidth="21705" windowHeight="12480" firstSheet="6" activeTab="13" xr2:uid="{9E3F4571-95A0-4D9B-935E-6906F522B3C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Carbohydrate" sheetId="7" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3481" uniqueCount="1649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3480" uniqueCount="1649">
   <si>
     <t/>
   </si>
@@ -4921,9 +4921,6 @@
     <t>PFK_3</t>
   </si>
   <si>
-    <t>Not added yet</t>
-  </si>
-  <si>
     <t>1.8.1.2</t>
   </si>
   <si>
@@ -4991,6 +4988,9 @@
   </si>
   <si>
     <t>Forward</t>
+  </si>
+  <si>
+    <t>BG_CELLB</t>
   </si>
 </sst>
 </file>
@@ -5517,8 +5517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEEC3A33-F582-43F5-91B0-F50E7298D19A}">
   <dimension ref="A1:L150"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="B146" sqref="B146"/>
+    <sheetView topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7147,7 +7147,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>950</v>
       </c>
@@ -7158,7 +7158,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>1071</v>
       </c>
@@ -7169,7 +7169,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>1620</v>
       </c>
@@ -7180,7 +7180,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>832</v>
       </c>
@@ -7190,11 +7190,8 @@
       <c r="D148" t="s">
         <v>153</v>
       </c>
-      <c r="E148" t="s">
-        <v>1625</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>80</v>
       </c>
@@ -7204,11 +7201,8 @@
       <c r="D149" t="s">
         <v>159</v>
       </c>
-      <c r="E149" t="s">
-        <v>1625</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>11</v>
       </c>
@@ -7217,9 +7211,6 @@
       </c>
       <c r="D150" t="s">
         <v>159</v>
-      </c>
-      <c r="E150" t="s">
-        <v>1625</v>
       </c>
     </row>
   </sheetData>
@@ -8684,7 +8675,7 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" s="30" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="D45" t="s">
         <v>1023</v>
@@ -8699,8 +8690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93A317DF-5D73-40B2-9988-3470DAE7D79F}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9235,10 +9226,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC83DB3-50B1-4EAD-BBE0-76DF2C07E3B2}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9262,14 +9253,14 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="B2" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -9277,7 +9268,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="D3" t="s">
         <v>528</v>
@@ -9296,10 +9287,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B5" t="s">
         <v>1629</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1630</v>
       </c>
       <c r="D5" t="s">
         <v>610</v>
@@ -9307,24 +9298,24 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="C6" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="D6" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
+        <v>1646</v>
+      </c>
+      <c r="C7" t="s">
         <v>1647</v>
       </c>
-      <c r="C7" t="s">
-        <v>1648</v>
-      </c>
       <c r="D7" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -9332,12 +9323,12 @@
         <v>1123</v>
       </c>
       <c r="D8" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="D9" t="s">
         <v>513</v>
@@ -9345,7 +9336,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="D10" t="s">
         <v>513</v>
@@ -9353,7 +9344,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="D11" t="s">
         <v>513</v>
@@ -9361,7 +9352,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="D12" t="s">
         <v>513</v>
@@ -9377,7 +9368,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="D14" t="s">
         <v>513</v>
@@ -9393,7 +9384,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="D16" t="s">
         <v>513</v>
@@ -9401,7 +9392,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="D17" t="s">
         <v>513</v>
@@ -9417,7 +9408,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="D19" t="s">
         <v>513</v>
@@ -9425,7 +9416,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="D20" t="s">
         <v>513</v>
@@ -9433,7 +9424,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D21" t="s">
         <v>513</v>
@@ -9441,7 +9432,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="D22" t="s">
         <v>513</v>
@@ -9449,10 +9440,18 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="D23" t="s">
         <v>513</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>1648</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1593</v>
       </c>
     </row>
   </sheetData>
@@ -9464,7 +9463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF454C2-0694-4E16-84A6-3AB2E62D53C7}">
   <dimension ref="A1:D159"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A142" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
@@ -11239,7 +11238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{934C3CA2-2D51-4F5B-82B7-15AD46F4E382}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -20050,7 +20049,7 @@
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="D100" t="s">
         <v>367</v>

</xml_diff>